<commit_message>
files with action collumn
</commit_message>
<xml_diff>
--- a/FonotradeInvoiceControlTests/files/one_person_registered.xlsx
+++ b/FonotradeInvoiceControlTests/files/one_person_registered.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">Lote</t>
   </si>
@@ -46,6 +46,18 @@
     <t xml:space="preserve">Valor</t>
   </si>
   <si>
+    <t xml:space="preserve">Ação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID REGISTRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID SERVIÇO</t>
+  </si>
+  <si>
     <t xml:space="preserve">220405-1</t>
   </si>
   <si>
@@ -59,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve">Curso de Aprimoramento On-line – Alfabetização e Fonoaudiologia Clínica: Interface saúde e educação - Abril/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CADASTRAR</t>
   </si>
   <si>
     <t xml:space="preserve">CADASTRADO</t>
@@ -118,7 +133,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -140,6 +155,13 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -166,7 +188,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -221,6 +243,10 @@
     </xf>
     <xf numFmtId="167" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -300,23 +326,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J1048576"/>
+  <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q3" activeCellId="0" sqref="Q3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="20.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="20.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="5.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="34.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="105.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="30.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="10.99"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="9" style="3" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="4.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="96.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="29.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="10.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="11.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="13.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="11.16"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="13" style="3" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -344,25 +374,37 @@
       <c r="H1" s="8" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B2" s="9" t="n">
         <v>1</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G2" s="12" t="str">
         <f aca="false">C2&amp;"-"&amp;A2&amp;"-"&amp;B2</f>
@@ -371,11 +413,17 @@
       <c r="H2" s="13" t="n">
         <v>350.22</v>
       </c>
-      <c r="I2" s="3" t="n">
+      <c r="I2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="10" t="n">
         <v>1234</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>13</v>
+      <c r="L2" s="10" t="n">
+        <v>4321</v>
       </c>
     </row>
     <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>